<commit_message>
Added Design Patterns Types Docs
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Docs_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8AAEC1-9BB5-4DEF-B5E7-6A6E216E9DB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3AA063-77B6-41B1-9DD5-713E795CB24E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="554" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="554" activeTab="1" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Career PATH_Arranged" sheetId="35" r:id="rId1"/>
@@ -2706,27 +2706,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2783,6 +2762,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3344,372 +3344,372 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="39" style="68" customWidth="1"/>
-    <col min="3" max="3" width="67.140625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" style="61" customWidth="1"/>
+    <col min="3" max="3" width="67.140625" style="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="68" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70">
+      <c r="A4" s="63">
         <v>1</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="77"/>
+      <c r="E4" s="70"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="65" t="s">
         <v>205</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="76"/>
-      <c r="E5" s="78"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="71"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>3</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="67" t="s">
         <v>206</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="76"/>
-      <c r="E6" s="78"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="71"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>4</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="67" t="s">
         <v>208</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="76"/>
-      <c r="E7" s="78"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="71"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>5</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="67" t="s">
         <v>210</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="78"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="71"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>6</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="67" t="s">
         <v>212</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="76"/>
-      <c r="E9" s="78"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="71"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>7</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="67" t="s">
         <v>218</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="78"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="71"/>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>8</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="67" t="s">
         <v>214</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="78"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="71"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>9</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="67" t="s">
         <v>216</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="78"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="71"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>10</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="65" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="76"/>
-      <c r="E13" s="78"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="71"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>11</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="76"/>
-      <c r="E14" s="78"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="71"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>12</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="65" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="76"/>
-      <c r="E15" s="78"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="71"/>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>13</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="65" t="s">
         <v>199</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="D16" s="71"/>
-      <c r="E16" s="78"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="71"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>14</v>
       </c>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="65" t="s">
         <v>200</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="78"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="71"/>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>15</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="65" t="s">
         <v>203</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D18" s="76"/>
-      <c r="E18" s="78"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="71"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>16</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="65" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="78"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="71"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>17</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="71"/>
-      <c r="E20" s="78"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="71"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>18</v>
       </c>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="76"/>
-      <c r="E21" s="78"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="71"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>19</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="76"/>
-      <c r="E22" s="78"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="71"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>20</v>
       </c>
-      <c r="B23" s="72" t="s">
+      <c r="B23" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="78"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="71"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>21</v>
       </c>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="65" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="76"/>
-      <c r="E24" s="78"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="71"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>22</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="65" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="76"/>
-      <c r="E25" s="78"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="71"/>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>23</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="76"/>
-      <c r="E26" s="78"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="71"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>1</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="55" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="14" t="s">
@@ -3723,10 +3723,10 @@
       <c r="A30" s="11">
         <v>2</v>
       </c>
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="62"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="1" t="s">
         <v>29</v>
       </c>
@@ -3735,7 +3735,7 @@
       <c r="A31" s="12">
         <v>3</v>
       </c>
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="61" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -3746,7 +3746,7 @@
       <c r="A32" s="11">
         <v>4</v>
       </c>
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="61" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -3810,14 +3810,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3880,14 +3880,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3933,9 +3933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27645D63-80B6-4CC9-9DF9-3EC673CAFE41}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3952,14 +3950,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4022,14 +4020,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4092,14 +4090,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4162,14 +4160,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4233,12 +4231,12 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
     </row>
@@ -4265,11 +4263,11 @@
       <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="39" t="s">
         <v>149</v>
       </c>
@@ -4565,12 +4563,12 @@
       <c r="A1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
       <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4596,11 +4594,11 @@
       <c r="A3" s="47">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
       <c r="E3" s="48" t="s">
         <v>150</v>
       </c>
@@ -4677,11 +4675,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="48" t="s">
         <v>150</v>
       </c>
@@ -4847,15 +4845,15 @@
   </sheetPr>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="39" style="69" customWidth="1"/>
-    <col min="3" max="3" width="67.140625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" style="62" customWidth="1"/>
+    <col min="3" max="3" width="67.140625" style="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
@@ -4864,35 +4862,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="52" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -4913,10 +4911,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="53" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="13" t="s">
@@ -4925,7 +4923,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="56" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -4937,10 +4935,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="53" t="s">
         <v>52</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -4949,7 +4947,7 @@
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="57" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4976,7 +4974,7 @@
       <c r="B9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="53" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -4985,10 +4983,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="56" t="s">
         <v>205</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="53" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -4997,7 +4995,7 @@
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="56" t="s">
         <v>206</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -5009,7 +5007,7 @@
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="56" t="s">
         <v>208</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -5021,7 +5019,7 @@
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="56" t="s">
         <v>210</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -5033,7 +5031,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="56" t="s">
         <v>212</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -5045,7 +5043,7 @@
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="56" t="s">
         <v>218</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -5057,7 +5055,7 @@
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="56" t="s">
         <v>214</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -5069,7 +5067,7 @@
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="56" t="s">
         <v>216</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -5096,7 +5094,7 @@
       <c r="B19" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="53" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="20" t="s">
@@ -5108,7 +5106,7 @@
       <c r="B20" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="53" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="20" t="s">
@@ -5120,7 +5118,7 @@
       <c r="B21" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="20" t="s">
@@ -5129,10 +5127,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="19" t="s">
@@ -5155,7 +5153,7 @@
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="59" t="s">
         <v>199</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -5167,7 +5165,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="59" t="s">
         <v>200</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -5179,7 +5177,7 @@
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="59" t="s">
         <v>203</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -5191,42 +5189,42 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
-      <c r="B27" s="67"/>
+      <c r="B27" s="60"/>
       <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
-      <c r="B28" s="67"/>
+      <c r="B28" s="60"/>
       <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
-      <c r="B29" s="67"/>
+      <c r="B29" s="60"/>
       <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
-      <c r="B30" s="67"/>
+      <c r="B30" s="60"/>
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="62" t="s">
+      <c r="C32" s="55" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="14" t="s">
@@ -5244,10 +5242,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="62" t="s">
+      <c r="C33" s="55" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -5256,7 +5254,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -5265,7 +5263,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
-      <c r="B35" s="68" t="s">
+      <c r="B35" s="61" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -5274,7 +5272,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
-      <c r="B36" s="68" t="s">
+      <c r="B36" s="61" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -5381,14 +5379,14 @@
       <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5448,14 +5446,14 @@
       <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5520,14 +5518,14 @@
       <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5590,13 +5588,13 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:8" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -5739,14 +5737,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5809,14 +5807,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5879,14 +5877,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5929,21 +5927,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d53f460e102142885dbc8938524af06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" xmlns:ns4="c8965576-7528-46e3-a68d-d4bc5141fdaa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51dd3132ab51039a0b8a02bab29c14ac" ns3:_="" ns4:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -6166,7 +6149,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC42E61D-1BC2-43F5-95E9-ABDA8B3BC8C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="df3f84f5-0dce-435a-abac-67420900ba59"/>
+    <ds:schemaRef ds:uri="c8965576-7528-46e3-a68d-d4bc5141fdaa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{236AB03D-89C6-4FEB-AC3B-BF68DD4F8BD0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -6183,29 +6200,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC37F108-450B-470C-B7B9-209E1FAF9670}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC42E61D-1BC2-43F5-95E9-ABDA8B3BC8C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="df3f84f5-0dce-435a-abac-67420900ba59"/>
-    <ds:schemaRef ds:uri="c8965576-7528-46e3-a68d-d4bc5141fdaa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>